<commit_message>
Fixed report download issue
</commit_message>
<xml_diff>
--- a/assessment_report.xlsx
+++ b/assessment_report.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="68">
   <si>
     <t>Monthly Exam 1 (15-Aug-2024)</t>
   </si>
@@ -194,6 +194,9 @@
   </si>
   <si>
     <t>C</t>
+  </si>
+  <si>
+    <t>U</t>
   </si>
   <si>
     <t>A</t>
@@ -1240,7 +1243,7 @@
         <v>42.86</v>
       </c>
       <c r="F34" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="35" spans="1:6">
@@ -1460,7 +1463,7 @@
         <v>85.70999999999999</v>
       </c>
       <c r="F45" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="46" spans="1:6">
@@ -1600,7 +1603,7 @@
         <v>57.14</v>
       </c>
       <c r="F52" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="53" spans="1:6">
@@ -1620,12 +1623,12 @@
         <v>51.43</v>
       </c>
       <c r="F53" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="56" spans="1:6">
       <c r="A56" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="57" spans="1:6">
@@ -1650,7 +1653,7 @@
     </row>
     <row r="58" spans="1:6">
       <c r="A58" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B58">
         <v>23</v>
@@ -2225,7 +2228,7 @@
         <v>42.86</v>
       </c>
       <c r="F86" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="87" spans="1:6">
@@ -2305,7 +2308,7 @@
         <v>45.71</v>
       </c>
       <c r="F90" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="91" spans="1:6">
@@ -2465,7 +2468,7 @@
         <v>74.29000000000001</v>
       </c>
       <c r="F98" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="99" spans="1:6">
@@ -2665,7 +2668,7 @@
         <v>74.29000000000001</v>
       </c>
       <c r="F108" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="109" spans="1:6">
@@ -2685,12 +2688,12 @@
         <v>74.29000000000001</v>
       </c>
       <c r="F109" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="112" spans="1:6">
       <c r="A112" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="113" spans="1:6">
@@ -2715,7 +2718,7 @@
     </row>
     <row r="114" spans="1:6">
       <c r="A114" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B114">
         <v>23</v>
@@ -3290,7 +3293,7 @@
         <v>57.14</v>
       </c>
       <c r="F142" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="143" spans="1:6">
@@ -3370,7 +3373,7 @@
         <v>45.71</v>
       </c>
       <c r="F146" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="147" spans="1:6">
@@ -3590,7 +3593,7 @@
         <v>85.70999999999999</v>
       </c>
       <c r="F157" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="158" spans="1:6">
@@ -3630,7 +3633,7 @@
         <v>42.86</v>
       </c>
       <c r="F159" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="160" spans="1:6">
@@ -3655,7 +3658,7 @@
     </row>
     <row r="161" spans="1:6">
       <c r="A161" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B161">
         <v>13399873</v>
@@ -3750,7 +3753,7 @@
         <v>57.14</v>
       </c>
       <c r="F165" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="166" spans="1:6">
@@ -3770,7 +3773,7 @@
         <v>71.43000000000001</v>
       </c>
       <c r="F166" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>